<commit_message>
smaller fixes to resume
</commit_message>
<xml_diff>
--- a/src/data/ansioluettelo.xlsx
+++ b/src/data/ansioluettelo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="440" windowWidth="24920" windowHeight="16360" tabRatio="500"/>
+    <workbookView xWindow="2560" yWindow="440" windowWidth="24920" windowHeight="16360" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Koulutus" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
   <si>
     <t>toimija</t>
   </si>
@@ -248,10 +248,13 @@
     <t>Otan laadukkaita valokuvia, jotka on optimoitu nettiin ja printtiin, käytän Canonin järjestelmäkameraa.</t>
   </si>
   <si>
-    <t>Olen työskennellyt suurten tietokantojen ja tietolähteiden kanssa. Esimerkiksi tietokannan siirto, web-karttatietojen käsittely (GeoJSON KML, SHP) tai kuvankäsittelyn automatisointi.</t>
-  </si>
-  <si>
     <t>Opintojeni suuntauksena oli Talous ja toimistopalvelut ja suoritin paljon yrittämiseen liittyviä kursseja. Opintoihini kuului kolme työharjoittelua palkanlaskenta yritys Silta Oy, Stockmann Oyj ja Ravintola-alan yritys Fonda Oy.</t>
+  </si>
+  <si>
+    <t>01/2014 - 06/2018</t>
+  </si>
+  <si>
+    <t>Olen työskennellyt suurten tietokantojen ja tietolähteiden kanssa. Esimerkiksi tietokannan siirto, web-karttatietojen käsittely (GeoJSON KML, SHP) js kuvankäsittelyn automatisointi.</t>
   </si>
 </sst>
 </file>
@@ -637,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -665,7 +668,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>61</v>
@@ -753,7 +756,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -811,7 +814,7 @@
         <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1020,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1071,7 +1074,7 @@
         <v>22</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
removed one thing from excel
</commit_message>
<xml_diff>
--- a/src/data/ansioluettelo.xlsx
+++ b/src/data/ansioluettelo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-37980" yWindow="920" windowWidth="24920" windowHeight="16360" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="-37980" yWindow="920" windowWidth="24920" windowHeight="16360" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Koulutus" sheetId="1" r:id="rId1"/>
@@ -194,9 +194,6 @@
     <t>Suunnittelen ja koodaan upeita verkkosivuja ja web-sovelluksia. Tiedän verkon parhaat käytännöt ja käytän sujuvasti HTML CSS, SCSS, Javascript, ES6, React ja Gatsby.js.</t>
   </si>
   <si>
-    <t>Perheyritys jossa olen työskennellyt ravintolan keittiössä ja auttanut johtoa IT- asioiden kanssa. Olen myös tehnyt ravintolan nykyiset verkkosivut.</t>
-  </si>
-  <si>
     <t>Tein kansainvälisestikin tunnetulle ravintolalle uudet verkkosivut ja autoin henkiökuntaa IT- asioissa ja sosiaalisen median kanssa.</t>
   </si>
   <si>
@@ -227,9 +224,6 @@
     <t>01/2014 - 06/2017</t>
   </si>
   <si>
-    <t>A family run business where I have worked in the restaurant's kitchen and helped magement with IT- issues. I have also done the existing website.</t>
-  </si>
-  <si>
     <t>I've made a globally recognized restaurant's website and helped staff with IT- issues and social media usage.</t>
   </si>
   <si>
@@ -252,6 +246,12 @@
   </si>
   <si>
     <t>01/2014 - 06/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perheyritys jossa olen työskennellyt ravintolan keittiössä ja auttanut johtoa IT- asioiden kanssa. </t>
+  </si>
+  <si>
+    <t>A family run business where I have worked in the restaurant's kitchen and helped magement with IT- issues.</t>
   </si>
 </sst>
 </file>
@@ -659,10 +659,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -670,13 +670,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="20" x14ac:dyDescent="0.2">
@@ -720,7 +720,7 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -728,13 +728,13 @@
         <v>29</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -747,7 +747,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -774,10 +774,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -788,10 +788,10 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -802,10 +802,10 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -819,7 +819,7 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -831,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -859,10 +859,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -873,10 +873,10 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -887,10 +887,10 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -904,7 +904,7 @@
         <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1014,7 +1014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="225" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1041,7 +1041,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="20" x14ac:dyDescent="0.2">
@@ -1073,7 +1073,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1112,7 +1112,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20" x14ac:dyDescent="0.2">
@@ -1120,7 +1120,7 @@
         <v>36</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="20" x14ac:dyDescent="0.2">

</xml_diff>